<commit_message>
added threading and optimization
</commit_message>
<xml_diff>
--- a/TableMetadata/metadata_excel.xlsx
+++ b/TableMetadata/metadata_excel.xlsx
@@ -31,7 +31,7 @@
     <t>T_EMP_ID</t>
   </si>
   <si>
-    <t>NUMBER(22)</t>
+    <t>int</t>
   </si>
   <si>
     <t>EMP_ID</t>
@@ -40,13 +40,13 @@
     <t>EMP_NAME</t>
   </si>
   <si>
-    <t>VARCHAR2(50)</t>
+    <t>varchar(50)</t>
   </si>
   <si>
     <t>DEPT_NAME</t>
   </si>
   <si>
-    <t>VARCHAR2(20)</t>
+    <t>varchar(20)</t>
   </si>
   <si>
     <t>MANAGER_NAME</t>
@@ -58,13 +58,13 @@
     <t>LOCATION</t>
   </si>
   <si>
-    <t>VARCHAR2(30)</t>
+    <t>varchar(30)</t>
   </si>
   <si>
     <t>HIRE_DATE</t>
   </si>
   <si>
-    <t>DATE</t>
+    <t>date</t>
   </si>
   <si>
     <t>TOTAL_EXP_IN_COMPANY</t>
@@ -82,7 +82,7 @@
     <t>SALARY_GRADE</t>
   </si>
   <si>
-    <t>VARCHAR2(10)</t>
+    <t>varchar(10)</t>
   </si>
   <si>
     <t>T_DEPT</t>
@@ -97,13 +97,13 @@
     <t>DNAME</t>
   </si>
   <si>
-    <t>VARCHAR2(14)</t>
+    <t>varchar(14)</t>
   </si>
   <si>
     <t>LOC</t>
   </si>
   <si>
-    <t>VARCHAR2(13)</t>
+    <t>varchar(13)</t>
   </si>
 </sst>
 </file>

</xml_diff>